<commit_message>
Part 2 Lessons 3-6
</commit_message>
<xml_diff>
--- a/excel_luke/2_Formulas_Functions/3_Logical_Functions.xlsx
+++ b/excel_luke/2_Formulas_Functions/3_Logical_Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liu_michael/Documents/UWaterloo1/Data Analytics/excel_luke/2_Formulas_Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DACF0C-E6D1-403B-A48D-03B483E33508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EACB95-BB4D-F840-9670-3D54E05A1D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-102" yWindow="1488" windowWidth="18372" windowHeight="10296" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
+    <workbookView xWindow="0" yWindow="1480" windowWidth="24600" windowHeight="14400" activeTab="2" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_1" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -580,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -861,12 +861,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,6 +972,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,37 +1337,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D423364-12D3-4C3A-8A6B-C3645EBFE927}">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="11.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26171875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.15625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.41796875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.68359375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.15625" style="1"/>
-    <col min="18" max="18" width="14.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25"/>
     </row>
-    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1400,7 +1416,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1457,9 +1473,12 @@
         <f>AND(L3,M3)</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="32"/>
-    </row>
-    <row r="4" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q3" s="32" t="str">
+        <f>IF(P3, "Goal Met", "Goal Not Met")</f>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1516,9 +1535,12 @@
         <f t="shared" ref="P4:P12" si="10">AND(L4,M4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="32"/>
-    </row>
-    <row r="5" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q4" s="32" t="str">
+        <f t="shared" ref="Q4:Q12" si="11">IF(P4, "Goal Met", "Goal Not Met")</f>
+        <v>Goal Not Met</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1575,9 +1597,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="32"/>
-    </row>
-    <row r="6" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q5" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Not Met</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1634,9 +1659,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="32"/>
-    </row>
-    <row r="7" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q6" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1693,9 +1721,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="32"/>
-    </row>
-    <row r="8" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q7" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Not Met</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1752,9 +1783,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="32"/>
-    </row>
-    <row r="9" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q8" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1811,9 +1845,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="32"/>
-    </row>
-    <row r="10" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q9" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1870,9 +1907,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="32"/>
-    </row>
-    <row r="11" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q10" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1929,9 +1969,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="32"/>
-    </row>
-    <row r="12" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q11" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Not Met</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -1988,14 +2031,17 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="33"/>
-    </row>
-    <row r="14" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q12" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>22</v>
       </c>
@@ -2003,7 +2049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>23</v>
       </c>
@@ -2024,33 +2070,33 @@
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="11.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.41796875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.68359375" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.68359375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.15625" style="1"/>
-    <col min="19" max="19" width="14.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" style="1"/>
+    <col min="19" max="19" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25"/>
     </row>
-    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +2146,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2162,7 +2208,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2224,7 +2270,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -2286,7 +2332,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -2348,7 +2394,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -2410,7 +2456,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -2472,7 +2518,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -2534,7 +2580,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -2596,7 +2642,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
@@ -2658,7 +2704,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -2720,12 +2766,12 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>22</v>
       </c>
@@ -2733,7 +2779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>23</v>
       </c>
@@ -2750,33 +2796,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18E6D21-2229-4383-8B9A-431F68FAE08C}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.15625" customWidth="1"/>
-    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="68.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.9453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.3125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.05078125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="68.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.5" customWidth="1"/>
+    <col min="16" max="16" width="0.1640625" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
@@ -2832,7 +2878,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
@@ -2863,8 +2909,32 @@
       <c r="J2" s="27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" t="str">
+        <f>IF($A2=K$1, "Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF($A2=L$1, "Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="M2" t="b">
+        <f>IF(OR(K2 = "Desired", L2 = "Desired"), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <f>AND($A2=$K$1, $A2=$L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <f>OR($A2=$K$1, $A2=$L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="str" cm="1">
+        <f t="array" ref="Q2">_xlfn.IFS($H2="", "No Data", $H2&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
@@ -2895,8 +2965,32 @@
       <c r="J3" s="27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:L21" si="0">IF($A3=K$1, "Desired", "Not Desired")</f>
+        <v>Desired</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M3" t="b">
+        <f t="shared" ref="M3:M21" si="1">IF(OR(K3 = "Desired", L3 = "Desired"), TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N3" t="b">
+        <f t="shared" ref="N3:N21" si="2">AND($A3=$K$1, $A3=$L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <f t="shared" ref="O3:O21" si="3">OR($A3=$K$1, $A3=$L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" t="str" cm="1">
+        <f t="array" ref="Q3">_xlfn.IFS($H3="", "No Data", $H3&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary Low</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
@@ -2925,8 +3019,32 @@
       <c r="J4" s="27" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M4" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" t="str" cm="1">
+        <f t="array" ref="Q4">_xlfn.IFS($H4="", "No Data", $H4&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
@@ -2955,8 +3073,32 @@
       <c r="J5" s="27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M5" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="str" cm="1">
+        <f t="array" ref="Q5">_xlfn.IFS($H5="", "No Data", $H5&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>76</v>
       </c>
@@ -2985,8 +3127,32 @@
       <c r="J6" s="27" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M6" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" t="str" cm="1">
+        <f t="array" ref="Q6">_xlfn.IFS($H6="", "No Data", $H6&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>0</v>
       </c>
@@ -3015,8 +3181,32 @@
       <c r="J7" s="27" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M7" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" t="str" cm="1">
+        <f t="array" ref="Q7">_xlfn.IFS($H7="", "No Data", $H7&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
@@ -3045,8 +3235,32 @@
       <c r="J8" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q8" t="str" cm="1">
+        <f t="array" ref="Q8">_xlfn.IFS($H8="", "No Data", $H8&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
@@ -3077,8 +3291,32 @@
       <c r="J9" s="27" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q9" t="str" cm="1">
+        <f t="array" ref="Q9">_xlfn.IFS($H9="", "No Data", $H9&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>2</v>
       </c>
@@ -3107,8 +3345,32 @@
       <c r="J10" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q10" t="str" cm="1">
+        <f t="array" ref="Q10">_xlfn.IFS($H10="", "No Data", $H10&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>2</v>
       </c>
@@ -3139,8 +3401,32 @@
       <c r="J11" s="27" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N11" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q11" t="str" cm="1">
+        <f t="array" ref="Q11">_xlfn.IFS($H11="", "No Data", $H11&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>0</v>
       </c>
@@ -3171,8 +3457,32 @@
       <c r="J12" s="27" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M12" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O12" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" t="str" cm="1">
+        <f t="array" ref="Q12">_xlfn.IFS($H12="", "No Data", $H12&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>102</v>
       </c>
@@ -3203,8 +3513,32 @@
       <c r="J13" s="27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" t="str" cm="1">
+        <f t="array" ref="Q13">_xlfn.IFS($H13="", "No Data", $H13&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>0</v>
       </c>
@@ -3235,8 +3569,32 @@
       <c r="J14" s="27" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" t="str" cm="1">
+        <f t="array" ref="Q14">_xlfn.IFS($H14="", "No Data", $H14&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>0</v>
       </c>
@@ -3267,8 +3625,32 @@
       <c r="J15" s="27" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" t="str" cm="1">
+        <f t="array" ref="Q15">_xlfn.IFS($H15="", "No Data", $H15&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary Low</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>4</v>
       </c>
@@ -3299,8 +3681,32 @@
       <c r="J16" s="27" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" t="str" cm="1">
+        <f t="array" ref="Q16">_xlfn.IFS($H16="", "No Data", $H16&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>4</v>
       </c>
@@ -3331,8 +3737,32 @@
       <c r="J17" s="27" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" t="str" cm="1">
+        <f t="array" ref="Q17">_xlfn.IFS($H17="", "No Data", $H17&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>123</v>
       </c>
@@ -3361,8 +3791,32 @@
       <c r="J18" s="27" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="M18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N18" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q18" t="str" cm="1">
+        <f t="array" ref="Q18">_xlfn.IFS($H18="", "No Data", $H18&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>0</v>
       </c>
@@ -3393,8 +3847,32 @@
       <c r="J19" s="27" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" t="str" cm="1">
+        <f t="array" ref="Q19">_xlfn.IFS($H19="", "No Data", $H19&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>0</v>
       </c>
@@ -3423,8 +3901,32 @@
       <c r="J20" s="27" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M20" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" t="str" cm="1">
+        <f t="array" ref="Q20">_xlfn.IFS($H20="", "No Data", $H20&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>123</v>
       </c>
@@ -3454,6 +3956,30 @@
       </c>
       <c r="J21" s="27" t="s">
         <v>135</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>Desired</v>
+      </c>
+      <c r="M21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N21" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" t="str" cm="1">
+        <f t="array" ref="Q21">_xlfn.IFS($H21="", "No Data", $H21&gt;$Q$1, "Salary &gt; 85k", TRUE, "Salary Low")</f>
+        <v>Salary &gt; 85k</v>
       </c>
     </row>
   </sheetData>
@@ -3467,29 +3993,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.41796875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83984375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="38.15625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="18.578125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="68.15625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="68.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
@@ -3549,7 +4075,7 @@
         <v>85000</v>
       </c>
     </row>
-    <row r="2" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
@@ -3613,7 +4139,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="3" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
@@ -3677,7 +4203,7 @@
         <v>Salary Low</v>
       </c>
     </row>
-    <row r="4" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
@@ -3739,7 +4265,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="5" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
@@ -3801,7 +4327,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="6" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>76</v>
       </c>
@@ -3863,7 +4389,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="7" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>0</v>
       </c>
@@ -3925,7 +4451,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="8" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
@@ -3987,7 +4513,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="9" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
@@ -4051,7 +4577,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="10" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>2</v>
       </c>
@@ -4113,7 +4639,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="11" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>2</v>
       </c>
@@ -4177,7 +4703,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="12" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>0</v>
       </c>
@@ -4241,7 +4767,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="13" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>102</v>
       </c>
@@ -4305,7 +4831,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="14" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>0</v>
       </c>
@@ -4369,7 +4895,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="15" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>0</v>
       </c>
@@ -4433,7 +4959,7 @@
         <v>Salary Low</v>
       </c>
     </row>
-    <row r="16" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>4</v>
       </c>
@@ -4497,7 +5023,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>4</v>
       </c>
@@ -4561,7 +5087,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>123</v>
       </c>
@@ -4623,7 +5149,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>0</v>
       </c>
@@ -4687,7 +5213,7 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>0</v>
       </c>
@@ -4749,7 +5275,7 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>123</v>
       </c>
@@ -4827,17 +5353,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.578125" customWidth="1"/>
-    <col min="2" max="2" width="13.41796875" customWidth="1"/>
-    <col min="3" max="3" width="31.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="26" t="s">
         <v>28</v>
       </c>
@@ -4854,7 +5380,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -4874,7 +5400,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="e">
         <f>A4 + "text"</f>
         <v>#VALUE!</v>
@@ -4894,7 +5420,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -4914,7 +5440,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="e" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">COUNTT(A3:A9)</f>
         <v>#NAME?</v>
@@ -4934,7 +5460,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="e">
         <f>VLOOKUP("Value", A1:A10, 2, FALSE)</f>
         <v>#N/A</v>
@@ -4954,7 +5480,7 @@
         <v>This hides #N/A error</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
@@ -4974,7 +5500,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="27" t="e">
         <f>SUM(A1:A10 C1:C10)</f>
         <v>#NULL!</v>
@@ -5003,18 +5529,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B83CC08-3BAC-45FD-A105-07186D54808A}">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="D2:E2"/>
+    <sheetView showGridLines="0" zoomScale="118" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.578125" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="36" t="s">
         <v>137</v>
       </c>
@@ -5028,7 +5554,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="38" t="b">
         <v>1</v>
       </c>
@@ -5044,7 +5570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="38" t="b">
         <v>1</v>
       </c>
@@ -5060,7 +5586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="38" t="b">
         <v>0</v>
       </c>
@@ -5076,7 +5602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="b">
         <v>0</v>
       </c>

</xml_diff>